<commit_message>
adapted test data to new minimal excel
</commit_message>
<xml_diff>
--- a/test/data/excel/minimal_cog.xlsx
+++ b/test/data/excel/minimal_cog.xlsx
@@ -89,7 +89,7 @@
     <t>PERSON1</t>
   </si>
   <si>
-    <t>/am/ (description) {anysource}</t>
+    <t>/am/ (A judgement comment) {anysource}</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
removed author of comment
</commit_message>
<xml_diff>
--- a/test/data/excel/minimal_cog.xlsx
+++ b/test/data/excel/minimal_cog.xlsx
@@ -25,23 +25,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>walter.fuchs:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-fictitious!</t>
+          <t>fictitious!</t>
         </r>
       </text>
     </comment>
@@ -96,7 +85,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,13 +108,6 @@
       <color rgb="FF000000"/>
       <name val="Cambria"/>
       <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -464,7 +446,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>

</xml_diff>